<commit_message>
up audit manque les ref
</commit_message>
<xml_diff>
--- a/0 - Livrables/Audit-SEO.xlsx
+++ b/0 - Livrables/Audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Samuel/Desktop/P4_Prigent_Samuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CD92F1-1134-EF46-8A21-74FFF3D7C583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F45C90-C155-AB48-9C7C-EAB790FD53B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="620" windowWidth="28760" windowHeight="17380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="122">
   <si>
     <t>Catégorie</t>
   </si>
@@ -357,6 +357,69 @@
   <si>
     <t>Bug de style résolus</t>
   </si>
+  <si>
+    <t>Alt</t>
+  </si>
+  <si>
+    <t>Mettre des alts sur les images précis et ne pas copier coller dans toutes les images le mêmes textes</t>
+  </si>
+  <si>
+    <t>Eviter les textes cachés car peu être perçu par le bot de google comme une mauvaise tentative dans le but d'augmenter son référencement induisant un maluse par ce bot</t>
+  </si>
+  <si>
+    <t>Compression</t>
+  </si>
+  <si>
+    <t>Minimifier</t>
+  </si>
+  <si>
+    <t>Minifier le css et le javascript en enlevenat les espaces et retour à la ligne permet d'améliorer la vitesse à laquelles ces fichiers seront lu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compresser les images et utiliser le source set pour charger des images différentes en fonction de la largeur de l'écran peu permettre de réduire de 90% la taille d'un dossier images.
+</t>
+  </si>
+  <si>
+    <t>defer</t>
+  </si>
+  <si>
+    <t>Utiliser defer sur des script javascript permet à la page de charger le style si ces scripts ne sont pas entièrement chargés</t>
+  </si>
+  <si>
+    <t>Constrate</t>
+  </si>
+  <si>
+    <t>Utiliser un logiciels pour vérifier que les contrastes soit valides au WCAG pour rendre le site accessible au plus grand nombre</t>
+  </si>
+  <si>
+    <t>Tabulation</t>
+  </si>
+  <si>
+    <t>Liens</t>
+  </si>
+  <si>
+    <t>Avoir une navigation possible et logique avec le clavier via la touche tab avec un changement de style lorsque l'élément est :focus avec un encadrement ou autre</t>
+  </si>
+  <si>
+    <t>Eviter les liens répétitifs sur la même pages car plus il y a de liens identique plus l'importance de ce liens diminue pour le référencement.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Avoir un titre pour chaque page html</t>
+  </si>
+  <si>
+    <t>Metadescription 
+&amp; Keywords</t>
+  </si>
+  <si>
+    <t>Avoir une metadescription avec des phrases claires allant à l'essentiel sans être répétitif.
+Et pour la balise de keywords utiliser des verbes d'actions différents sans répéter les mêmes mots.</t>
+  </si>
+  <si>
+    <t>Textes cachés</t>
+  </si>
 </sst>
 </file>
 
@@ -495,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -542,7 +605,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,6 +633,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,7 +881,7 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>59</v>
       </c>
       <c r="E1" s="2"/>
@@ -849,7 +917,7 @@
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -859,28 +927,28 @@
         <v>40</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
     </row>
     <row r="5" spans="1:23" ht="40" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -890,28 +958,28 @@
         <v>41</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
     </row>
     <row r="6" spans="1:23" ht="40" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -919,28 +987,28 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
     </row>
     <row r="7" spans="1:23" ht="40" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -951,7 +1019,7 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -965,7 +1033,7 @@
       </c>
     </row>
     <row r="9" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -977,7 +1045,7 @@
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:23" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -988,7 +1056,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -999,7 +1067,7 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="80" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1013,7 +1081,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" s="6" customFormat="1" ht="40" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -1025,7 +1093,7 @@
       <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="12"/>
@@ -1039,7 +1107,7 @@
       <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:23" ht="40" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1050,7 +1118,7 @@
       </c>
     </row>
     <row r="17" spans="1:16384" ht="60" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1064,7 +1132,7 @@
       </c>
     </row>
     <row r="18" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -1075,7 +1143,7 @@
       </c>
     </row>
     <row r="19" spans="1:16384" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1086,7 +1154,7 @@
       </c>
     </row>
     <row r="20" spans="1:16384" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="14" t="s">
@@ -1096,28 +1164,28 @@
         <v>91</v>
       </c>
       <c r="D20" s="15"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
     </row>
     <row r="21" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1128,7 +1196,7 @@
       </c>
     </row>
     <row r="22" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -1139,7 +1207,7 @@
       </c>
     </row>
     <row r="23" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1150,7 +1218,7 @@
       </c>
     </row>
     <row r="24" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1161,7 +1229,7 @@
       </c>
     </row>
     <row r="25" spans="1:16384" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -1171,8 +1239,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:16384" ht="60" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -1183,7 +1251,7 @@
       </c>
     </row>
     <row r="27" spans="1:16384" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
     </row>
@@ -17576,7 +17644,7 @@
       <c r="XFD28" s="10"/>
     </row>
     <row r="29" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -17587,7 +17655,7 @@
       </c>
     </row>
     <row r="30" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -17598,7 +17666,7 @@
       </c>
     </row>
     <row r="31" spans="1:16384" ht="40" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -17609,7 +17677,7 @@
       </c>
     </row>
     <row r="32" spans="1:16384" ht="60" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B32" s="9" t="s">
@@ -17632,7 +17700,7 @@
       <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:4" s="8" customFormat="1" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -17644,7 +17712,7 @@
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="13" t="s">
@@ -17655,7 +17723,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="140" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -17666,7 +17734,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="140" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -17677,7 +17745,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -17688,7 +17756,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -17699,7 +17767,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="40" x14ac:dyDescent="0.2">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -17710,7 +17778,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="40" x14ac:dyDescent="0.2">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -17721,7 +17789,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -17732,7 +17800,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="40" x14ac:dyDescent="0.2">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -17743,7 +17811,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="9" t="s">
@@ -17754,7 +17822,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="9" t="s">
@@ -17765,7 +17833,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="40" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B47" s="9" t="s">
@@ -17776,7 +17844,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B48" s="9" t="s">
@@ -17787,7 +17855,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -17798,22 +17866,22 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="22"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="22"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="22"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
     </row>
@@ -18258,14 +18326,14 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="88.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="116.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -18298,75 +18366,115 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
+      <c r="B3" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="72" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="B8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>115</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="B9" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" ht="23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>